<commit_message>
updated input data file to reduce its size
</commit_message>
<xml_diff>
--- a/annex_vi_clp_table_atp18_en.xlsx
+++ b/annex_vi_clp_table_atp18_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stach\Desktop\exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177C0CB9-2778-4E59-BE38-450AA97F423D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F38446C-6FC9-4E68-811E-2DB45BC6DD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2045,8 +2045,8 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N25" sqref="N25"/>
+      <pane ySplit="6" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>